<commit_message>
can create excel and fixed SEVERAL BUGS
</commit_message>
<xml_diff>
--- a/src/public/template.xlsx
+++ b/src/public/template.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Results" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Ponderaciones" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -165,13 +165,10 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:N2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -217,7 +214,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.3" right="0.3" top="0.609722222222222" bottom="0.370138888888889" header="0.1" footer="0.1"/>

</xml_diff>

<commit_message>
Fixed hour and university on excel
</commit_message>
<xml_diff>
--- a/src/public/template.xlsx
+++ b/src/public/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Ponderaciones" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">nombre</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t xml:space="preserve">carrera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">universidad</t>
   </si>
   <si>
     <t xml:space="preserve">hora</t>
@@ -162,15 +165,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -213,15 +219,10 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.3" right="0.3" top="0.609722222222222" bottom="0.370138888888889" header="0.1" footer="0.1"/>

</xml_diff>